<commit_message>
daily commit, iterate to week
</commit_message>
<xml_diff>
--- a/stalist.xlsx
+++ b/stalist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucinda/Downloads/Data Download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926FACD7-B4FE-E747-85D2-B5E5390F9B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4FDD66-8235-344D-9CF2-1C340406BC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="5300" windowWidth="44480" windowHeight="17440" xr2:uid="{DA0E83F3-D192-8E49-B619-AE0883EFAF53}"/>
   </bookViews>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5412463E-0CE7-404A-81B8-F1505AD7D9DD}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1661,182 +1661,50 @@
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-    </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-    </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-    </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-    </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-    </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-    </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-    </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-    </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-    </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-    </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-    </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-    </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-    </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-    </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-    </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-    </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-    </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-    </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
-    </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C124" s="1"/>
-      <c r="D124" s="1"/>
-    </row>
+    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>